<commit_message>
novas bases de dados
</commit_message>
<xml_diff>
--- a/Urbanizacao censo 2010 v0.xlsx
+++ b/Urbanizacao censo 2010 v0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="15140" windowHeight="9300"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="15135" windowHeight="9300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="base de dados hom" sheetId="2" r:id="rId1"/>
@@ -780,21 +780,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.1796875" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="6.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.36328125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="40" customHeight="1">
+    <row r="1" spans="1:6" ht="39.950000000000003" customHeight="1">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -814,7 +814,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="12.5">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -831,7 +831,7 @@
         <v>733559</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="12.5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -848,7 +848,7 @@
         <v>3120494</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="12.5">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -865,7 +865,7 @@
         <v>3483985</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="12.5">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -882,7 +882,7 @@
         <v>669526</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="12.5">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -899,7 +899,7 @@
         <v>14016906</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="12.5">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -916,7 +916,7 @@
         <v>8452381</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="12.5">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -933,7 +933,7 @@
         <v>2570160</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="12.5">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -950,7 +950,7 @@
         <v>3514952</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="12.5">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -967,7 +967,7 @@
         <v>6003788</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="12.5">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -984,7 +984,7 @@
         <v>6574789</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="12.5">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>19597330</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="12.5">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>2449024</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="12.5">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>3035122</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="12.5">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>7581051</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="12.5">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>3766528</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="12.5">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>8796448</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="12.5">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>3110292</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="12.5">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>10444526</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="12.5">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>15989929</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="12.5">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>3168027</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="12.5">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>63</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>1562409</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="12.5">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>450479</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="12.5">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>10693929</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="12.5">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>6248436</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="12.5">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>2068017</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="12.5">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>41262199</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="12.5">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>81</v>
       </c>
@@ -1298,23 +1298,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.1796875" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="6.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="17" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.36328125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="3" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="40" customHeight="1">
+    <row r="1" spans="1:11" ht="39.950000000000003" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="12.5">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1358,7 +1358,7 @@
       </c>
       <c r="G2" s="11"/>
     </row>
-    <row r="3" spans="1:11" ht="12.5">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1379,7 +1379,7 @@
       </c>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:11" ht="12.5">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:11" ht="12.5">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1421,7 +1421,7 @@
       </c>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:11" ht="13">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="12.5">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1470,7 +1470,7 @@
       </c>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" ht="12.5">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:11" ht="12.5">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1520,7 +1520,7 @@
       </c>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:11" ht="12.5">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:11" ht="12.5">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1570,7 +1570,7 @@
       </c>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11" ht="12.5">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1591,7 +1591,7 @@
       </c>
       <c r="G12" s="11"/>
     </row>
-    <row r="13" spans="1:11" ht="12.5">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1612,7 +1612,7 @@
       </c>
       <c r="G13" s="11"/>
     </row>
-    <row r="14" spans="1:11" ht="12.5">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1633,7 +1633,7 @@
       </c>
       <c r="G14" s="11"/>
     </row>
-    <row r="15" spans="1:11" ht="12.5">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1654,7 +1654,7 @@
       </c>
       <c r="G15" s="11"/>
     </row>
-    <row r="16" spans="1:11" ht="12.5">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="G16" s="11"/>
     </row>
-    <row r="17" spans="1:7" ht="12.5">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="G17" s="11"/>
     </row>
-    <row r="18" spans="1:7" ht="12.5">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -1717,7 +1717,7 @@
       </c>
       <c r="G18" s="11"/>
     </row>
-    <row r="19" spans="1:7" ht="12.5">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -1738,7 +1738,7 @@
       </c>
       <c r="G19" s="11"/>
     </row>
-    <row r="20" spans="1:7" ht="12.5">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -1759,7 +1759,7 @@
       </c>
       <c r="G20" s="11"/>
     </row>
-    <row r="21" spans="1:7" ht="12.5">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -1780,7 +1780,7 @@
       </c>
       <c r="G21" s="11"/>
     </row>
-    <row r="22" spans="1:7" ht="12.5">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>69</v>
       </c>
@@ -1801,7 +1801,7 @@
       </c>
       <c r="G22" s="11"/>
     </row>
-    <row r="23" spans="1:7" ht="12.5">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -1822,7 +1822,7 @@
       </c>
       <c r="G23" s="11"/>
     </row>
-    <row r="24" spans="1:7" ht="12.5">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -1843,7 +1843,7 @@
       </c>
       <c r="G24" s="11"/>
     </row>
-    <row r="25" spans="1:7" ht="12.5">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -1864,7 +1864,7 @@
       </c>
       <c r="G25" s="11"/>
     </row>
-    <row r="26" spans="1:7" ht="12.5">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>78</v>
       </c>
@@ -1885,7 +1885,7 @@
       </c>
       <c r="G26" s="11"/>
     </row>
-    <row r="27" spans="1:7" ht="12.5">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>75</v>
       </c>
@@ -1906,7 +1906,7 @@
       </c>
       <c r="G27" s="11"/>
     </row>
-    <row r="28" spans="1:7" ht="12.5">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>81</v>
       </c>

</xml_diff>